<commit_message>
lines experiment, reordering files
</commit_message>
<xml_diff>
--- a/ThesisDocument/Pictures_list.xlsx
+++ b/ThesisDocument/Pictures_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raulleal/Documents/DogTime/year 5/DogtimeThesis/ThesisDocument/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raula\Documents\DogtimeThesis\ThesisDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ED77D9-73E9-0A4A-8534-01DDDE122122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9424AED3-5035-4E82-A4D3-A6ABDAB85212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22040" yWindow="500" windowWidth="22040" windowHeight="14340" xr2:uid="{F705D91A-7E53-2446-8868-DC18BEF6EFD8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{F705D91A-7E53-2446-8868-DC18BEF6EFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>Work of art</t>
   </si>
@@ -318,12 +318,27 @@
   <si>
     <t>https://digitalartmuseum.org/gallery/image/8847.html</t>
   </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Poster_Salon_Soci%C3%A9t%C3%A9_nationale_des_beaux-arts_Paris_1891.png</t>
+  </si>
+  <si>
+    <t>Salon des beaux arts</t>
+  </si>
+  <si>
+    <t>https://www.artsy.net/artwork/sturtevant-dapres-martial-raysse-peinture-a-haute-tension</t>
+  </si>
+  <si>
+    <t>Raysse</t>
+  </si>
+  <si>
+    <t>stedelijk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,6 +371,14 @@
       <color rgb="FF757575"/>
       <name val="Neutral Regular 3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -374,10 +397,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,8 +409,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -699,13 +725,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5637075-DE1F-1141-8A6D-CB1C3ECEA35B}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -726,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22">
+    <row r="2" spans="1:5" ht="21">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -754,7 +780,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17">
+    <row r="4" spans="1:5" ht="16.5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -764,14 +790,14 @@
       <c r="C4">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17">
+    <row r="5" spans="1:5" ht="16.5">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -795,384 +821,409 @@
       <c r="C6">
         <v>14</v>
       </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>17</v>
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>17</v>
+      <c r="D9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
       <c r="C12">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17.5">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>81</v>
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
       <c r="C16">
         <v>24</v>
       </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C18">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C19">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C22">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
       </c>
       <c r="C24">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C25">
-        <v>35</v>
-      </c>
-      <c r="D25" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="D26" t="s">
-        <v>85</v>
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
       </c>
       <c r="C27">
         <v>35</v>
       </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28">
-        <v>39</v>
+      <c r="D28" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C29">
-        <v>40</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C30">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C31">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
       </c>
       <c r="C32">
-        <v>49</v>
-      </c>
-      <c r="D32" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
       </c>
       <c r="C33">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34">
         <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C35">
         <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36">
         <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37">
         <v>49</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C38">
         <v>49</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C39">
         <v>49</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>79</v>
+      <c r="D39" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="C40">
+        <v>49</v>
+      </c>
+      <c r="D40" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41">
+        <v>49</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>62</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{73629CA2-C640-4CBF-B823-57FAA0351830}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>